<commit_message>
Edited Git Commands in Excel Sheet
</commit_message>
<xml_diff>
--- a/05. GIT/GIT COMMANDS.xlsx
+++ b/05. GIT/GIT COMMANDS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Git Commands</t>
   </si>
@@ -127,6 +127,18 @@
   <si>
     <t>git checkout Branch-Name</t>
   </si>
+  <si>
+    <t>git clone Gihtub-Project-Link</t>
+  </si>
+  <si>
+    <t>git remote add origin Github-Project-Link</t>
+  </si>
+  <si>
+    <t>To clone the repo into your local machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attach your local repo to Github Repo </t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,7 +438,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -927,8 +942,12 @@
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="2:24" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -952,8 +971,12 @@
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="2:24" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>

</xml_diff>